<commit_message>
committing final bbref data for 2014-2018 all teams
</commit_message>
<xml_diff>
--- a/Project Luther Features.xlsx
+++ b/Project Luther Features.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17600" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="198">
   <si>
     <t>W-L (ordinal)</t>
   </si>
@@ -169,13 +170,466 @@
   </si>
   <si>
     <t>Miami</t>
+  </si>
+  <si>
+    <t>ATL</t>
+  </si>
+  <si>
+    <t>ARI</t>
+  </si>
+  <si>
+    <t>BAL</t>
+  </si>
+  <si>
+    <t>BOS</t>
+  </si>
+  <si>
+    <t>CHC</t>
+  </si>
+  <si>
+    <t>CHW</t>
+  </si>
+  <si>
+    <t>CIN</t>
+  </si>
+  <si>
+    <t>CLE</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t>DET</t>
+  </si>
+  <si>
+    <t>KCR</t>
+  </si>
+  <si>
+    <t>HOU</t>
+  </si>
+  <si>
+    <t>LAA</t>
+  </si>
+  <si>
+    <t>LAD</t>
+  </si>
+  <si>
+    <t>MIA</t>
+  </si>
+  <si>
+    <t>MIL</t>
+  </si>
+  <si>
+    <t>MIN</t>
+  </si>
+  <si>
+    <t>NYM</t>
+  </si>
+  <si>
+    <t>NYY</t>
+  </si>
+  <si>
+    <t>OAK</t>
+  </si>
+  <si>
+    <t>PHI</t>
+  </si>
+  <si>
+    <t>PIT</t>
+  </si>
+  <si>
+    <t>SDP</t>
+  </si>
+  <si>
+    <t>SEA</t>
+  </si>
+  <si>
+    <t>SFG</t>
+  </si>
+  <si>
+    <t>STL</t>
+  </si>
+  <si>
+    <t>TBR</t>
+  </si>
+  <si>
+    <t>TEX</t>
+  </si>
+  <si>
+    <t>TOR</t>
+  </si>
+  <si>
+    <t>WSN</t>
+  </si>
+  <si>
+    <t>ATL_2015 = bbrs.pullTableATL, 2015</t>
+  </si>
+  <si>
+    <t>[ATL_2015, ARI_2015, BAL_2015, BOS_2015, CHC_2015, CHW_2015, CIN_2015, CLE_2015, COL_2015, DET_2015, KCR_2015, HOU_2015, LAA_2015, LAD_2015, MIA_2015, MIL_2015, MIN_2015, NYM_2015, NYY_2015, OAK_2015, PHI_2015, PIT_2015, SDP_2015, SEA_2015, SFG_2015, STL_2015, TBR_2015, TEX_2015, TOR_2015, WSN_2015, ATL_2016, ARI_2016, BAL_2016, BOS_2016, CHC_2016, CHW_2016, CIN_2016, CLE_2016, COL_2016, DET_2016, KCR_2016, HOU_2016, LAA_2016, LAD_2016, MIA_2016, MIL_2016, MIN_2016, NYM_2016, NYY_2016, OAK_2016, PHI_2016, PIT_2016, SDP_2016, SEA_2016, SFG_2016, STL_2016, TBR_2016, TEX_2016, TOR_2016, WSN_2016, ATL_2017, ARI_2017, BAL_2017, BOS_2017, CHC_2017, CHW_2017, CIN_2017, CLE_2017, COL_2017, DET_2017, KCR_2017, HOU_2017, LAA_2017, LAD_2017, MIA_2017, MIL_2017, MIN_2017, NYM_2017, NYY_2017, OAK_2017, PHI_2017, PIT_2017, SDP_2017, SEA_2017, SFG_2017, STL_2017, TBR_2017, TEX_2017, TOR_2017, WSN_2017, ATL_2018, ARI_2018, BAL_2018, BOS_2018, CHC_2018, CHW_2018, CIN_2018, CLE_2018, COL_2018, DET_2018, KCR_2018, HOU_2018, LAA_2018, LAD_2018, MIA_2018, MIL_2018, MIN_2018, NYM_2018, NYY_2018, OAK_2018, PHI_2018, PIT_2018, SDP_2018, SEA_2018, SFG_2018, STL_2018, TBR_2018, TEX_2018, TOR_2018, WSN_2018]</t>
+  </si>
+  <si>
+    <t>ARI_2015 = bbrs.pullTableARI, 2015</t>
+  </si>
+  <si>
+    <t>BAL_2015 = bbrs.pullTableBAL, 2015</t>
+  </si>
+  <si>
+    <t>BOS_2015 = bbrs.pullTableBOS, 2015</t>
+  </si>
+  <si>
+    <t>CHC_2015 = bbrs.pullTableCHC, 2015</t>
+  </si>
+  <si>
+    <t>CHW_2015 = bbrs.pullTableCHW, 2015</t>
+  </si>
+  <si>
+    <t>CIN_2015 = bbrs.pullTableCIN, 2015</t>
+  </si>
+  <si>
+    <t>CLE_2015 = bbrs.pullTableCLE, 2015</t>
+  </si>
+  <si>
+    <t>COL_2015 = bbrs.pullTableCOL, 2015</t>
+  </si>
+  <si>
+    <t>DET_2015 = bbrs.pullTableDET, 2015</t>
+  </si>
+  <si>
+    <t>KCR_2015 = bbrs.pullTableKCR, 2015</t>
+  </si>
+  <si>
+    <t>HOU_2015 = bbrs.pullTableHOU, 2015</t>
+  </si>
+  <si>
+    <t>LAA_2015 = bbrs.pullTableLAA, 2015</t>
+  </si>
+  <si>
+    <t>LAD_2015 = bbrs.pullTableLAD, 2015</t>
+  </si>
+  <si>
+    <t>MIA_2015 = bbrs.pullTableMIA, 2015</t>
+  </si>
+  <si>
+    <t>MIL_2015 = bbrs.pullTableMIL, 2015</t>
+  </si>
+  <si>
+    <t>MIN_2015 = bbrs.pullTableMIN, 2015</t>
+  </si>
+  <si>
+    <t>NYM_2015 = bbrs.pullTableNYM, 2015</t>
+  </si>
+  <si>
+    <t>NYY_2015 = bbrs.pullTableNYY, 2015</t>
+  </si>
+  <si>
+    <t>OAK_2015 = bbrs.pullTableOAK, 2015</t>
+  </si>
+  <si>
+    <t>PHI_2015 = bbrs.pullTablePHI, 2015</t>
+  </si>
+  <si>
+    <t>PIT_2015 = bbrs.pullTablePIT, 2015</t>
+  </si>
+  <si>
+    <t>SDP_2015 = bbrs.pullTableSDP, 2015</t>
+  </si>
+  <si>
+    <t>SEA_2015 = bbrs.pullTableSEA, 2015</t>
+  </si>
+  <si>
+    <t>SFG_2015 = bbrs.pullTableSFG, 2015</t>
+  </si>
+  <si>
+    <t>STL_2015 = bbrs.pullTableSTL, 2015</t>
+  </si>
+  <si>
+    <t>TBR_2015 = bbrs.pullTableTBR, 2015</t>
+  </si>
+  <si>
+    <t>TEX_2015 = bbrs.pullTableTEX, 2015</t>
+  </si>
+  <si>
+    <t>TOR_2015 = bbrs.pullTableTOR, 2015</t>
+  </si>
+  <si>
+    <t>WSN_2015 = bbrs.pullTableWSN, 2015</t>
+  </si>
+  <si>
+    <t>ATL_2016 = bbrs.pullTableATL, 2016</t>
+  </si>
+  <si>
+    <t>ARI_2016 = bbrs.pullTableARI, 2016</t>
+  </si>
+  <si>
+    <t>BAL_2016 = bbrs.pullTableBAL, 2016</t>
+  </si>
+  <si>
+    <t>BOS_2016 = bbrs.pullTableBOS, 2016</t>
+  </si>
+  <si>
+    <t>CHC_2016 = bbrs.pullTableCHC, 2016</t>
+  </si>
+  <si>
+    <t>CHW_2016 = bbrs.pullTableCHW, 2016</t>
+  </si>
+  <si>
+    <t>CIN_2016 = bbrs.pullTableCIN, 2016</t>
+  </si>
+  <si>
+    <t>CLE_2016 = bbrs.pullTableCLE, 2016</t>
+  </si>
+  <si>
+    <t>COL_2016 = bbrs.pullTableCOL, 2016</t>
+  </si>
+  <si>
+    <t>DET_2016 = bbrs.pullTableDET, 2016</t>
+  </si>
+  <si>
+    <t>KCR_2016 = bbrs.pullTableKCR, 2016</t>
+  </si>
+  <si>
+    <t>HOU_2016 = bbrs.pullTableHOU, 2016</t>
+  </si>
+  <si>
+    <t>LAA_2016 = bbrs.pullTableLAA, 2016</t>
+  </si>
+  <si>
+    <t>LAD_2016 = bbrs.pullTableLAD, 2016</t>
+  </si>
+  <si>
+    <t>MIA_2016 = bbrs.pullTableMIA, 2016</t>
+  </si>
+  <si>
+    <t>MIL_2016 = bbrs.pullTableMIL, 2016</t>
+  </si>
+  <si>
+    <t>MIN_2016 = bbrs.pullTableMIN, 2016</t>
+  </si>
+  <si>
+    <t>NYM_2016 = bbrs.pullTableNYM, 2016</t>
+  </si>
+  <si>
+    <t>NYY_2016 = bbrs.pullTableNYY, 2016</t>
+  </si>
+  <si>
+    <t>OAK_2016 = bbrs.pullTableOAK, 2016</t>
+  </si>
+  <si>
+    <t>PHI_2016 = bbrs.pullTablePHI, 2016</t>
+  </si>
+  <si>
+    <t>PIT_2016 = bbrs.pullTablePIT, 2016</t>
+  </si>
+  <si>
+    <t>SDP_2016 = bbrs.pullTableSDP, 2016</t>
+  </si>
+  <si>
+    <t>SEA_2016 = bbrs.pullTableSEA, 2016</t>
+  </si>
+  <si>
+    <t>SFG_2016 = bbrs.pullTableSFG, 2016</t>
+  </si>
+  <si>
+    <t>STL_2016 = bbrs.pullTableSTL, 2016</t>
+  </si>
+  <si>
+    <t>TBR_2016 = bbrs.pullTableTBR, 2016</t>
+  </si>
+  <si>
+    <t>TEX_2016 = bbrs.pullTableTEX, 2016</t>
+  </si>
+  <si>
+    <t>TOR_2016 = bbrs.pullTableTOR, 2016</t>
+  </si>
+  <si>
+    <t>WSN_2016 = bbrs.pullTableWSN, 2016</t>
+  </si>
+  <si>
+    <t>ATL_2017 = bbrs.pullTableATL, 2017</t>
+  </si>
+  <si>
+    <t>ARI_2017 = bbrs.pullTableARI, 2017</t>
+  </si>
+  <si>
+    <t>BAL_2017 = bbrs.pullTableBAL, 2017</t>
+  </si>
+  <si>
+    <t>BOS_2017 = bbrs.pullTableBOS, 2017</t>
+  </si>
+  <si>
+    <t>CHC_2017 = bbrs.pullTableCHC, 2017</t>
+  </si>
+  <si>
+    <t>CHW_2017 = bbrs.pullTableCHW, 2017</t>
+  </si>
+  <si>
+    <t>CIN_2017 = bbrs.pullTableCIN, 2017</t>
+  </si>
+  <si>
+    <t>CLE_2017 = bbrs.pullTableCLE, 2017</t>
+  </si>
+  <si>
+    <t>COL_2017 = bbrs.pullTableCOL, 2017</t>
+  </si>
+  <si>
+    <t>DET_2017 = bbrs.pullTableDET, 2017</t>
+  </si>
+  <si>
+    <t>KCR_2017 = bbrs.pullTableKCR, 2017</t>
+  </si>
+  <si>
+    <t>HOU_2017 = bbrs.pullTableHOU, 2017</t>
+  </si>
+  <si>
+    <t>LAA_2017 = bbrs.pullTableLAA, 2017</t>
+  </si>
+  <si>
+    <t>LAD_2017 = bbrs.pullTableLAD, 2017</t>
+  </si>
+  <si>
+    <t>MIA_2017 = bbrs.pullTableMIA, 2017</t>
+  </si>
+  <si>
+    <t>MIL_2017 = bbrs.pullTableMIL, 2017</t>
+  </si>
+  <si>
+    <t>MIN_2017 = bbrs.pullTableMIN, 2017</t>
+  </si>
+  <si>
+    <t>NYM_2017 = bbrs.pullTableNYM, 2017</t>
+  </si>
+  <si>
+    <t>NYY_2017 = bbrs.pullTableNYY, 2017</t>
+  </si>
+  <si>
+    <t>OAK_2017 = bbrs.pullTableOAK, 2017</t>
+  </si>
+  <si>
+    <t>PHI_2017 = bbrs.pullTablePHI, 2017</t>
+  </si>
+  <si>
+    <t>PIT_2017 = bbrs.pullTablePIT, 2017</t>
+  </si>
+  <si>
+    <t>SDP_2017 = bbrs.pullTableSDP, 2017</t>
+  </si>
+  <si>
+    <t>SEA_2017 = bbrs.pullTableSEA, 2017</t>
+  </si>
+  <si>
+    <t>SFG_2017 = bbrs.pullTableSFG, 2017</t>
+  </si>
+  <si>
+    <t>STL_2017 = bbrs.pullTableSTL, 2017</t>
+  </si>
+  <si>
+    <t>TBR_2017 = bbrs.pullTableTBR, 2017</t>
+  </si>
+  <si>
+    <t>TEX_2017 = bbrs.pullTableTEX, 2017</t>
+  </si>
+  <si>
+    <t>TOR_2017 = bbrs.pullTableTOR, 2017</t>
+  </si>
+  <si>
+    <t>WSN_2017 = bbrs.pullTableWSN, 2017</t>
+  </si>
+  <si>
+    <t>ATL_2018 = bbrs.pullTableATL, 2018</t>
+  </si>
+  <si>
+    <t>ARI_2018 = bbrs.pullTableARI, 2018</t>
+  </si>
+  <si>
+    <t>BAL_2018 = bbrs.pullTableBAL, 2018</t>
+  </si>
+  <si>
+    <t>BOS_2018 = bbrs.pullTableBOS, 2018</t>
+  </si>
+  <si>
+    <t>CHC_2018 = bbrs.pullTableCHC, 2018</t>
+  </si>
+  <si>
+    <t>CHW_2018 = bbrs.pullTableCHW, 2018</t>
+  </si>
+  <si>
+    <t>CIN_2018 = bbrs.pullTableCIN, 2018</t>
+  </si>
+  <si>
+    <t>CLE_2018 = bbrs.pullTableCLE, 2018</t>
+  </si>
+  <si>
+    <t>COL_2018 = bbrs.pullTableCOL, 2018</t>
+  </si>
+  <si>
+    <t>DET_2018 = bbrs.pullTableDET, 2018</t>
+  </si>
+  <si>
+    <t>KCR_2018 = bbrs.pullTableKCR, 2018</t>
+  </si>
+  <si>
+    <t>HOU_2018 = bbrs.pullTableHOU, 2018</t>
+  </si>
+  <si>
+    <t>LAA_2018 = bbrs.pullTableLAA, 2018</t>
+  </si>
+  <si>
+    <t>LAD_2018 = bbrs.pullTableLAD, 2018</t>
+  </si>
+  <si>
+    <t>MIA_2018 = bbrs.pullTableMIA, 2018</t>
+  </si>
+  <si>
+    <t>MIL_2018 = bbrs.pullTableMIL, 2018</t>
+  </si>
+  <si>
+    <t>MIN_2018 = bbrs.pullTableMIN, 2018</t>
+  </si>
+  <si>
+    <t>NYM_2018 = bbrs.pullTableNYM, 2018</t>
+  </si>
+  <si>
+    <t>NYY_2018 = bbrs.pullTableNYY, 2018</t>
+  </si>
+  <si>
+    <t>OAK_2018 = bbrs.pullTableOAK, 2018</t>
+  </si>
+  <si>
+    <t>PHI_2018 = bbrs.pullTablePHI, 2018</t>
+  </si>
+  <si>
+    <t>PIT_2018 = bbrs.pullTablePIT, 2018</t>
+  </si>
+  <si>
+    <t>SDP_2018 = bbrs.pullTableSDP, 2018</t>
+  </si>
+  <si>
+    <t>SEA_2018 = bbrs.pullTableSEA, 2018</t>
+  </si>
+  <si>
+    <t>SFG_2018 = bbrs.pullTableSFG, 2018</t>
+  </si>
+  <si>
+    <t>STL_2018 = bbrs.pullTableSTL, 2018</t>
+  </si>
+  <si>
+    <t>TBR_2018 = bbrs.pullTableTBR, 2018</t>
+  </si>
+  <si>
+    <t>TEX_2018 = bbrs.pullTableTEX, 2018</t>
+  </si>
+  <si>
+    <t>TOR_2018 = bbrs.pullTableTOR, 2018</t>
+  </si>
+  <si>
+    <t>WSN_2018 = bbrs.pullTableWSN, 2018</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -218,13 +672,25 @@
       <name val="Helvetica"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Monaco"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -240,7 +706,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -255,6 +721,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -535,7 +1005,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
@@ -773,6 +1243,1353 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J127"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="10">
+        <v>2015</v>
+      </c>
+      <c r="C1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C10" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C12" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C13" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C14" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C15" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C16" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C17" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B18" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B19" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C20" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C21" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C22" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B23" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C23" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B24" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C24" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B25" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C25" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B26" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C26" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B27" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C27" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B28" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C28" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B29" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C29" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B30" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C30" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B31" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C31" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B32" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C32" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B33" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C33" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B34" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C34" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B35" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C35" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B36" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C36" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B37" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C37" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B38" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C38" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B39" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C39" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B40" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C40" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B41" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C41" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B42" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C42" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B43" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C43" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B44" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C44" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B45" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C45" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B46" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C46" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B47" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C47" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B48" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C48" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B49" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C49" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B50" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C50" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B51" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C51" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B52" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C52" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B53" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C53" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B54" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C54" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B55" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C55" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B56" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C56" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B57" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C57" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B58" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C58" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B59" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C59" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B60" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C60" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B61" s="1">
+        <v>2017</v>
+      </c>
+      <c r="C61" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B62" s="1">
+        <v>2017</v>
+      </c>
+      <c r="C62" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B63" s="1">
+        <v>2017</v>
+      </c>
+      <c r="C63" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B64" s="1">
+        <v>2017</v>
+      </c>
+      <c r="C64" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B65" s="1">
+        <v>2017</v>
+      </c>
+      <c r="C65" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B66" s="1">
+        <v>2017</v>
+      </c>
+      <c r="C66" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B67" s="1">
+        <v>2017</v>
+      </c>
+      <c r="C67" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B68" s="1">
+        <v>2017</v>
+      </c>
+      <c r="C68" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B69" s="1">
+        <v>2017</v>
+      </c>
+      <c r="C69" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B70" s="1">
+        <v>2017</v>
+      </c>
+      <c r="C70" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B71" s="1">
+        <v>2017</v>
+      </c>
+      <c r="C71" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B72" s="1">
+        <v>2017</v>
+      </c>
+      <c r="C72" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B73" s="1">
+        <v>2017</v>
+      </c>
+      <c r="C73" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B74" s="1">
+        <v>2017</v>
+      </c>
+      <c r="C74" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B75" s="1">
+        <v>2017</v>
+      </c>
+      <c r="C75" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B76" s="1">
+        <v>2017</v>
+      </c>
+      <c r="C76" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B77" s="1">
+        <v>2017</v>
+      </c>
+      <c r="C77" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B78" s="1">
+        <v>2017</v>
+      </c>
+      <c r="C78" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B79" s="1">
+        <v>2017</v>
+      </c>
+      <c r="C79" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B80" s="1">
+        <v>2017</v>
+      </c>
+      <c r="C80" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B81" s="1">
+        <v>2017</v>
+      </c>
+      <c r="C81" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B82" s="1">
+        <v>2017</v>
+      </c>
+      <c r="C82" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A83" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B83" s="1">
+        <v>2017</v>
+      </c>
+      <c r="C83" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B84" s="1">
+        <v>2017</v>
+      </c>
+      <c r="C84" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A85" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B85" s="1">
+        <v>2017</v>
+      </c>
+      <c r="C85" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B86" s="1">
+        <v>2017</v>
+      </c>
+      <c r="C86" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B87" s="1">
+        <v>2017</v>
+      </c>
+      <c r="C87" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A88" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B88" s="1">
+        <v>2017</v>
+      </c>
+      <c r="C88" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A89" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B89" s="1">
+        <v>2017</v>
+      </c>
+      <c r="C89" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A90" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B90" s="1">
+        <v>2017</v>
+      </c>
+      <c r="C90" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A91" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B91" s="1">
+        <v>2018</v>
+      </c>
+      <c r="C91" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A92" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B92" s="1">
+        <v>2018</v>
+      </c>
+      <c r="C92" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A93" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B93" s="1">
+        <v>2018</v>
+      </c>
+      <c r="C93" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A94" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B94" s="1">
+        <v>2018</v>
+      </c>
+      <c r="C94" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A95" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B95" s="1">
+        <v>2018</v>
+      </c>
+      <c r="C95" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A96" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B96" s="1">
+        <v>2018</v>
+      </c>
+      <c r="C96" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A97" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B97" s="1">
+        <v>2018</v>
+      </c>
+      <c r="C97" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A98" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B98" s="1">
+        <v>2018</v>
+      </c>
+      <c r="C98" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A99" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B99" s="1">
+        <v>2018</v>
+      </c>
+      <c r="C99" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A100" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B100" s="1">
+        <v>2018</v>
+      </c>
+      <c r="C100" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A101" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B101" s="1">
+        <v>2018</v>
+      </c>
+      <c r="C101" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A102" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B102" s="1">
+        <v>2018</v>
+      </c>
+      <c r="C102" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A103" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B103" s="1">
+        <v>2018</v>
+      </c>
+      <c r="C103" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A104" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B104" s="1">
+        <v>2018</v>
+      </c>
+      <c r="C104" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A105" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B105" s="1">
+        <v>2018</v>
+      </c>
+      <c r="C105" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A106" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B106" s="1">
+        <v>2018</v>
+      </c>
+      <c r="C106" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A107" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B107" s="1">
+        <v>2018</v>
+      </c>
+      <c r="C107" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A108" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B108" s="1">
+        <v>2018</v>
+      </c>
+      <c r="C108" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A109" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B109" s="1">
+        <v>2018</v>
+      </c>
+      <c r="C109" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A110" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B110" s="1">
+        <v>2018</v>
+      </c>
+      <c r="C110" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A111" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B111" s="1">
+        <v>2018</v>
+      </c>
+      <c r="C111" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A112" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B112" s="1">
+        <v>2018</v>
+      </c>
+      <c r="C112" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A113" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B113" s="1">
+        <v>2018</v>
+      </c>
+      <c r="C113" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A114" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B114" s="1">
+        <v>2018</v>
+      </c>
+      <c r="C114" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A115" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B115" s="1">
+        <v>2018</v>
+      </c>
+      <c r="C115" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A116" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B116" s="1">
+        <v>2018</v>
+      </c>
+      <c r="C116" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A117" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B117" s="1">
+        <v>2018</v>
+      </c>
+      <c r="C117" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A118" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B118" s="1">
+        <v>2018</v>
+      </c>
+      <c r="C118" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A119" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B119" s="1">
+        <v>2018</v>
+      </c>
+      <c r="C119" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A120" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B120" s="1">
+        <v>2018</v>
+      </c>
+      <c r="C120" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G127">
+        <f>19436/120</f>
+        <v>161.96666666666667</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L16"/>
   <sheetViews>

</xml_diff>